<commit_message>
concept defualt 3 fixed: lf multiplied by 8760
</commit_message>
<xml_diff>
--- a/default/3_sut_multi_year_rcot_cap/concept.xlsx
+++ b/default/3_sut_multi_year_rcot_cap/concept.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MIMO\pyESM\default\3_sut_multi_year_rcot_cap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3_sut_multi_year_rcot_cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D45E49D-3D9E-40E1-8315-E3565A1A2FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0973B1-99FF-453B-817F-DEBFA1771E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -734,10 +734,10 @@
   <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="AA46" sqref="AA46"/>
+      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1568,7 @@
         <v>24</v>
       </c>
       <c r="J32">
-        <f t="array" ref="J32:L36">N32:P36*J17:L17</f>
+        <f t="array" ref="J32:L36">N32:P36*J17:L17*8760</f>
         <v>0</v>
       </c>
       <c r="K32">
@@ -1736,14 +1736,14 @@
         <v>24</v>
       </c>
       <c r="J39">
-        <f t="array" ref="J39:L43">N32:P36*J18:L18</f>
-        <v>156.35178999999999</v>
+        <f t="array" ref="J39:L43">N32:P36*J18:L18*8760</f>
+        <v>1369641.6804</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>508022.2</v>
+        <v>4450274472</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -1751,13 +1751,13 @@
         <v>25</v>
       </c>
       <c r="J40">
-        <v>156.35178999999999</v>
+        <v>1369641.6804</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>518182.64399999997</v>
+        <v>4539279961.4399996</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>26</v>
       </c>
       <c r="J41">
-        <v>156.35178999999999</v>
+        <v>1369641.6804</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>528546.29680000001</v>
+        <v>4630065559.9680004</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -1779,13 +1779,13 @@
         <v>27</v>
       </c>
       <c r="J42">
-        <v>187.83930339999998</v>
+        <v>1645472.2977839997</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>539117.22279999999</v>
+        <v>4722666871.7279997</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -1793,13 +1793,13 @@
         <v>28</v>
       </c>
       <c r="J43">
-        <v>224.75569829999998</v>
+        <v>1968859.9171079998</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>549899.56720000005</v>
+        <v>4817120208.6720009</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
conceptual model 3 with disposal capacity
</commit_message>
<xml_diff>
--- a/default/3_sut_multi_year_rcot_cap/concept.xlsx
+++ b/default/3_sut_multi_year_rcot_cap/concept.xlsx
@@ -8,111 +8,161 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3_sut_multi_year_rcot_cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D482DB9-8A2E-4AE1-83B9-B03DE1292D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C134AB13-0B9A-40D6-A6CE-81B84A79D127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no disposal" sheetId="2" r:id="rId1"/>
-    <sheet name="disposal" sheetId="3" r:id="rId2"/>
+    <sheet name="disposal_mat" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="disposal" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">disposal!$F$27:$H$31,disposal!$N$27:$P$31,disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">disposal!$F$27:$H$31,disposal!$N$27:$P$31,disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31,disposal_mat!$N$27:$P$31,disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28,'no disposal'!$N$24:$P$28,'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">disposal!$AD$10:$AH$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">disposal!$Z$10:$AD$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">disposal_mat!$AD$10:$AH$12</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'no disposal'!$Z$10:$AD$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">disposal!$F$27:$H$31</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">disposal!$F$27:$H$31</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">disposal!$J$34:$L$38</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">disposal!$J$34:$L$38</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">disposal_mat!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'no disposal'!$J$32:$L$36</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">disposal!$AD$7:$AH$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">disposal!$Z$7:$AD$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">disposal_mat!$AD$7:$AH$8</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'no disposal'!$Z$7:$AD$8</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">disposal!$X$14</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">disposal!$T$14</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">disposal_mat!$X$14</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'no disposal'!$T$14</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">disposal!$J$41:$L$45</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">disposal!$J$41:$L$45</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">disposal_mat!$J$41:$L$45</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'no disposal'!$J$39:$L$43</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
@@ -137,7 +187,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -159,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="104">
   <si>
     <t>time</t>
   </si>
@@ -402,6 +452,75 @@
   </si>
   <si>
     <t>Cap_new_diag</t>
+  </si>
+  <si>
+    <t>flows_agg/flows</t>
+  </si>
+  <si>
+    <t>Minimize(sum(C_inv,C_om))</t>
+  </si>
+  <si>
+    <t>C_inv = Cap_new * diag(c_inv)</t>
+  </si>
+  <si>
+    <t>c_inv</t>
+  </si>
+  <si>
+    <t>c_om</t>
+  </si>
+  <si>
+    <t>emiss</t>
+  </si>
+  <si>
+    <t>lf_min</t>
+  </si>
+  <si>
+    <t>lf_max</t>
+  </si>
+  <si>
+    <t>weib_shape</t>
+  </si>
+  <si>
+    <t>lt_avg</t>
+  </si>
+  <si>
+    <t>C_om = X * diag(c_om)</t>
+  </si>
+  <si>
+    <t>Cap_disp_new_t = weib_t * Cap_new_t</t>
+  </si>
+  <si>
+    <t>Cap_disp_start = c_start weib_concat</t>
+  </si>
+  <si>
+    <t>weib t.1 new</t>
+  </si>
+  <si>
+    <t>weib t.2 new</t>
+  </si>
+  <si>
+    <t>weib t.3 new</t>
+  </si>
+  <si>
+    <t>weib_start t.1</t>
+  </si>
+  <si>
+    <t>weib_start t.2</t>
+  </si>
+  <si>
+    <t>weib_start t.3</t>
+  </si>
+  <si>
+    <t>Xmin = Cap_op * diag(lf_min) * 8760</t>
+  </si>
+  <si>
+    <t>Xmin = Cap_op * diag(lf_max) * 8760</t>
+  </si>
+  <si>
+    <t>C_start</t>
+  </si>
+  <si>
+    <t>Cap_op = c_start + Tyy*Cap_new + Tyy*Cap_disp_new + Tyy*Cap_disp_start</t>
   </si>
 </sst>
 </file>
@@ -562,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -593,15 +712,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +1005,10 @@
   <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y22" sqref="Y22"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,17 +2188,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F83180C-7F37-49BA-8D43-1CE2099A28F0}">
   <dimension ref="A1:BG69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N34" sqref="N34"/>
+      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="6.42578125" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
     <col min="10" max="12" width="6.85546875" customWidth="1"/>
@@ -2131,7 +2254,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -2162,7 +2285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="76.5" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -2172,18 +2295,10 @@
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2506,7 +2621,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="J14" s="2">
         <v>10</v>
@@ -2522,7 +2637,7 @@
       </c>
       <c r="X14" s="15">
         <f>SUM(R27:T31,R34:T38)</f>
-        <v>2651871.5226486097</v>
+        <v>2651877.8847193602</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -2533,7 +2648,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="J15" s="2">
         <v>10</v>
@@ -2553,7 +2668,7 @@
         <v>23</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="J16" s="2">
         <v>50</v>
@@ -2573,7 +2688,7 @@
         <v>30</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="J17" s="2">
         <v>0</v>
@@ -2590,7 +2705,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="J18" s="2">
         <v>0.7</v>
@@ -2623,7 +2738,7 @@
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D20" s="32" t="s">
+      <c r="D20" t="s">
         <v>66</v>
       </c>
       <c r="E20" t="s">
@@ -2643,14 +2758,14 @@
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D21" s="32" t="s">
+      <c r="D21" t="s">
         <v>65</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="J21" s="2">
         <v>3</v>
@@ -2663,14 +2778,14 @@
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D22" s="32" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="J22" s="2">
         <v>3</v>
@@ -2708,9 +2823,9 @@
         <v>38</v>
       </c>
       <c r="R25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="X25" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="X25" s="26" t="s">
         <v>70</v>
       </c>
       <c r="AS25" t="s">
@@ -2760,7 +2875,7 @@
       <c r="T26" t="s">
         <v>35</v>
       </c>
-      <c r="W26" s="30" t="s">
+      <c r="W26" s="28" t="s">
         <v>71</v>
       </c>
       <c r="X26" s="9">
@@ -2883,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="18">
-        <v>1.9280932</v>
+        <v>2.2711823</v>
       </c>
       <c r="R27">
         <f t="array" ref="R27:T31">MMULT(N27:P31,_xlfn.MUNIT(3)*J14:L14)</f>
@@ -2893,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <v>9.640466</v>
+        <v>11.355911499999999</v>
       </c>
       <c r="W27" s="12">
         <v>1</v>
@@ -3024,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="20">
-        <v>0.22711716000000001</v>
+        <v>0.48419723999999997</v>
       </c>
       <c r="R28">
         <v>0.11305076999999999</v>
@@ -3033,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <v>1.1355858000000001</v>
+        <v>2.4209861999999998</v>
       </c>
       <c r="W28" s="12">
         <v>2</v>
@@ -3164,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="20">
-        <v>0.59219697999999998</v>
+        <v>0.71276614999999999</v>
       </c>
       <c r="R29">
         <v>0.17112985</v>
@@ -3173,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>2.9609848999999997</v>
+        <v>3.5638307500000002</v>
       </c>
       <c r="W29" s="12">
         <v>3</v>
@@ -3307,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="20">
-        <v>1.0412059</v>
+        <v>1.1765669999999999</v>
       </c>
       <c r="R30">
         <v>0.20431115999999999</v>
@@ -3316,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>5.2060294999999996</v>
+        <v>5.882835</v>
       </c>
       <c r="W30" s="12">
         <v>4</v>
@@ -3453,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="23">
-        <v>1.1092594</v>
+        <v>1.5255741</v>
       </c>
       <c r="R31">
         <v>0.24059423999999999</v>
@@ -3462,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>5.546297</v>
+        <v>7.6278705000000002</v>
       </c>
       <c r="W31" s="12">
         <v>5</v>
@@ -3574,15 +3689,15 @@
       </c>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="P32" s="28"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J33" s="14" t="s">
@@ -3596,30 +3711,18 @@
       </c>
       <c r="Q33" s="14"/>
       <c r="R33" s="14" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="S33" s="14"/>
-      <c r="X33" s="29" t="s">
+      <c r="X33" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="Y33" s="31"/>
-      <c r="Z33" s="31"/>
-      <c r="AA33" s="31"/>
-      <c r="AB33" s="31"/>
-      <c r="AE33" s="29" t="s">
+      <c r="AE33" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AF33" s="31"/>
-      <c r="AG33" s="31"/>
-      <c r="AH33" s="31"/>
-      <c r="AI33" s="31"/>
-      <c r="AL33" s="29" t="s">
+      <c r="AL33" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="AM33" s="31"/>
-      <c r="AN33" s="31"/>
-      <c r="AO33" s="31"/>
-      <c r="AP33" s="31"/>
       <c r="AS33" s="14" t="s">
         <v>79</v>
       </c>
@@ -3645,8 +3748,8 @@
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="P34" s="26">
-        <v>0.37096340326565647</v>
+      <c r="P34">
+        <v>0.37151217019214017</v>
       </c>
       <c r="R34">
         <f t="array" ref="R34:T38">MMULT(J27:L31,_xlfn.MUNIT(3)*J15:L15)</f>
@@ -3714,8 +3817,8 @@
       <c r="O35">
         <v>0</v>
       </c>
-      <c r="P35" s="26">
-        <v>0.41709903925052216</v>
+      <c r="P35">
+        <v>0.42620383690416558</v>
       </c>
       <c r="R35">
         <v>1302.9315999999999</v>
@@ -3779,8 +3882,8 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="P36" s="26">
-        <v>0.60576802064019319</v>
+      <c r="P36">
+        <v>0.65361288295800191</v>
       </c>
       <c r="R36">
         <v>1563.5178999999998</v>
@@ -3844,8 +3947,8 @@
       <c r="O37">
         <v>0</v>
       </c>
-      <c r="P37" s="26">
-        <v>0.98086951864194583</v>
+      <c r="P37">
+        <v>1.116230631545081</v>
       </c>
       <c r="R37">
         <v>1878.3931000000002</v>
@@ -3909,8 +4012,8 @@
       <c r="O38">
         <v>0</v>
       </c>
-      <c r="P38" s="26">
-        <v>1.2433845328364463</v>
+      <c r="P38">
+        <v>1.4640310399418639</v>
       </c>
       <c r="R38">
         <v>2247.5569999999998</v>
@@ -3977,7 +4080,7 @@
         <v>0</v>
       </c>
       <c r="L41">
-        <v>448009.14038785704</v>
+        <v>508022.20674233703</v>
       </c>
       <c r="N41">
         <f t="array" ref="N41:P45">J19:L19-MMULT(N48:R52,N34:P38)+MMULT(N48:R52,N27:P31)</f>
@@ -3987,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="P41">
-        <v>2.5571297967343436</v>
+        <v>2.89967012980786</v>
       </c>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.25">
@@ -4001,7 +4104,7 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <v>414724.31514316553</v>
+        <v>518182.65096472722</v>
       </c>
       <c r="N42">
         <v>2.1248069339576355E-2</v>
@@ -4010,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="P42">
-        <v>2.3671479174838215</v>
+        <v>2.9576635329036942</v>
       </c>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.25">
@@ -4024,7 +4127,7 @@
         <v>0</v>
       </c>
       <c r="L43">
-        <v>412346.66882300359</v>
+        <v>528546.30335048528</v>
       </c>
       <c r="N43">
         <v>2.5497683371895591E-2</v>
@@ -4033,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>2.3535768768436278</v>
+        <v>3.0168167999456923</v>
       </c>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.25">
@@ -4047,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <v>422917.60283693462</v>
+        <v>539117.23510378716</v>
       </c>
       <c r="N44">
         <v>3.0632632914770114E-2</v>
@@ -4056,7 +4159,7 @@
         <v>0</v>
       </c>
       <c r="P44">
-        <v>2.4139132582016818</v>
+        <v>3.0771531684006117</v>
       </c>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.25">
@@ -4070,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="L45">
-        <v>399418.87956398918</v>
+        <v>549899.57922597264</v>
       </c>
       <c r="N45">
         <v>3.6652919231234399E-2</v>
@@ -4079,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="P45">
-        <v>2.279788125365235</v>
+        <v>3.1386962284587483</v>
       </c>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.25">
@@ -4188,7 +4291,7 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N54" s="29" t="s">
+      <c r="N54" s="27" t="s">
         <v>80</v>
       </c>
       <c r="O54" s="9"/>
@@ -4315,7 +4418,7 @@
       </c>
       <c r="P65" cm="1">
         <f t="array" ref="P65:P69">P27:P31</f>
-        <v>1.9280932</v>
+        <v>2.2711823</v>
       </c>
     </row>
     <row r="66" spans="14:16" x14ac:dyDescent="0.25">
@@ -4326,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="P66">
-        <v>0.22711716000000001</v>
+        <v>0.48419723999999997</v>
       </c>
     </row>
     <row r="67" spans="14:16" x14ac:dyDescent="0.25">
@@ -4337,7 +4440,7 @@
         <v>0</v>
       </c>
       <c r="P67">
-        <v>0.59219697999999998</v>
+        <v>0.71276614999999999</v>
       </c>
     </row>
     <row r="68" spans="14:16" x14ac:dyDescent="0.25">
@@ -4348,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="P68">
-        <v>1.0412059</v>
+        <v>1.1765669999999999</v>
       </c>
     </row>
     <row r="69" spans="14:16" x14ac:dyDescent="0.25">
@@ -4359,10 +4462,1933 @@
         <v>0</v>
       </c>
       <c r="P69">
-        <v>1.1092594</v>
+        <v>1.5255741</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F067AF8-4B71-42B5-9201-A885A5FCA9EF}">
+  <dimension ref="A1:AU52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="X24" sqref="X24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="12" width="6.85546875" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="16" width="7.42578125" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" customWidth="1"/>
+    <col min="20" max="32" width="7.42578125" customWidth="1"/>
+    <col min="33" max="34" width="4.85546875" customWidth="1"/>
+    <col min="35" max="35" width="5.28515625" customWidth="1"/>
+    <col min="36" max="38" width="7.140625" customWidth="1"/>
+    <col min="39" max="43" width="5.28515625" customWidth="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>2</v>
+      </c>
+      <c r="P1">
+        <v>3</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>5</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <v>2</v>
+      </c>
+      <c r="V1">
+        <v>3</v>
+      </c>
+      <c r="W1">
+        <v>4</v>
+      </c>
+      <c r="X1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="J6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF6" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>100</v>
+      </c>
+      <c r="O7" s="3">
+        <v>120</v>
+      </c>
+      <c r="P7" s="3">
+        <v>144</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>173</v>
+      </c>
+      <c r="R7" s="3">
+        <v>207</v>
+      </c>
+      <c r="T7">
+        <f t="array" ref="T7:X8">MMULT(AF7:AH8,TRANSPOSE(F27:H31))</f>
+        <v>108.57763</v>
+      </c>
+      <c r="U7">
+        <v>130.29316</v>
+      </c>
+      <c r="V7">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="W7">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="X7">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="Z7" s="13">
+        <f t="array" ref="Z7:AD8">T7:X8-MMULT(J7:L8,TRANSPOSE(J27:L31))-N7:R8</f>
+        <v>-2.7699999947117249E-6</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>3.6000000136482413E-7</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>-1.4100000100825127E-6</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>4.5099999965714233E-6</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>-3.0000001061125658E-7</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>508022.19999999995</v>
+      </c>
+      <c r="O8" s="3">
+        <v>518182.64399999997</v>
+      </c>
+      <c r="P8" s="3">
+        <v>528546.29687999992</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>539117.22281759989</v>
+      </c>
+      <c r="R8" s="3">
+        <v>549899.56727395195</v>
+      </c>
+      <c r="T8">
+        <v>508022.2</v>
+      </c>
+      <c r="U8">
+        <v>518182.64</v>
+      </c>
+      <c r="V8">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="W8">
+        <v>539117.22</v>
+      </c>
+      <c r="X8">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>-3.9999999571591616E-3</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>3.1200001249089837E-3</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>-2.8175999177619815E-3</v>
+      </c>
+      <c r="AD8" s="10">
+        <v>2.7260479982942343E-3</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Z10" s="5">
+        <f t="array" ref="Z10:AD12">TRANSPOSE(J27:L31)-MMULT(F10:H12,TRANSPOSE(F27:H31))</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Z11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Z12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="T13" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="2">
+        <v>10</v>
+      </c>
+      <c r="K14" s="2">
+        <v>10</v>
+      </c>
+      <c r="L14" s="2">
+        <v>5</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="T14" s="15">
+        <f>SUM(R27:T31,R34:T38)</f>
+        <v>2651877.8847193602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="2">
+        <v>10</v>
+      </c>
+      <c r="K15" s="2">
+        <v>10</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="2">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
+        <v>5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="2">
+        <v>3</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="2">
+        <v>3</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="X24" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE24" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL24" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="X25" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>11</v>
+      </c>
+      <c r="O26" t="s">
+        <v>18</v>
+      </c>
+      <c r="P26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R26" t="s">
+        <v>11</v>
+      </c>
+      <c r="S26" t="s">
+        <v>18</v>
+      </c>
+      <c r="T26" t="s">
+        <v>35</v>
+      </c>
+      <c r="W26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="X26" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE26" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI26" s="9">
+        <v>5</v>
+      </c>
+      <c r="AL26" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM26" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP26" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29">
+        <v>108.57763</v>
+      </c>
+      <c r="G27" s="29">
+        <v>0</v>
+      </c>
+      <c r="H27" s="29">
+        <v>508022.2</v>
+      </c>
+      <c r="I27" s="30"/>
+      <c r="J27" s="29">
+        <v>108.57763</v>
+      </c>
+      <c r="K27" s="29">
+        <v>0</v>
+      </c>
+      <c r="L27" s="29">
+        <v>508022.2</v>
+      </c>
+      <c r="M27" s="30"/>
+      <c r="N27" s="29">
+        <v>1.9829939000000001E-2</v>
+      </c>
+      <c r="O27" s="29">
+        <v>0</v>
+      </c>
+      <c r="P27" s="29">
+        <v>2.2711823</v>
+      </c>
+      <c r="R27">
+        <f t="array" ref="R27:T31">MMULT(N27:P31,_xlfn.MUNIT(3)*J14:L14)</f>
+        <v>0.19829939000000002</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>11.355911499999999</v>
+      </c>
+      <c r="W27" s="12">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W27),J$22,J$21,FALSE)</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="5">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W27),K$22,K$21,FALSE)</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="5">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W27),L$22,L$21,FALSE)</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="29">
+        <v>130.29316</v>
+      </c>
+      <c r="G28" s="29">
+        <v>0</v>
+      </c>
+      <c r="H28" s="29">
+        <v>518182.64</v>
+      </c>
+      <c r="I28" s="30"/>
+      <c r="J28" s="29">
+        <v>130.29316</v>
+      </c>
+      <c r="K28" s="29">
+        <v>0</v>
+      </c>
+      <c r="L28" s="29">
+        <v>518182.64</v>
+      </c>
+      <c r="M28" s="30"/>
+      <c r="N28" s="29">
+        <v>1.1305077E-2</v>
+      </c>
+      <c r="O28" s="29">
+        <v>0</v>
+      </c>
+      <c r="P28" s="29">
+        <v>0.48419723999999997</v>
+      </c>
+      <c r="R28">
+        <v>0.11305076999999999</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>2.4209861999999998</v>
+      </c>
+      <c r="W28" s="12">
+        <v>2</v>
+      </c>
+      <c r="X28">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W28),J$22,J$21,FALSE)</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="Y28">
+        <f>X27</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W28),K$22,K$21,FALSE)</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AF28">
+        <f>AE27</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AG28">
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W28),L$22,L$21,FALSE)</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AM28">
+        <f>AL27</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AN28">
+        <v>0</v>
+      </c>
+      <c r="AO28">
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="F29" s="29">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="G29" s="29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="29">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="29">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="K29" s="29">
+        <v>0</v>
+      </c>
+      <c r="L29" s="29">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="M29" s="30"/>
+      <c r="N29" s="29">
+        <v>1.7112985000000001E-2</v>
+      </c>
+      <c r="O29" s="29">
+        <v>0</v>
+      </c>
+      <c r="P29" s="29">
+        <v>0.71276614999999999</v>
+      </c>
+      <c r="R29">
+        <v>0.17112985</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>3.5638307500000002</v>
+      </c>
+      <c r="W29" s="12">
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W29),J$22,J$21,FALSE)</f>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Z31" si="0">X28</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="Z29">
+        <f>Y28</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W29),K$22,K$21,FALSE)</f>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" ref="AF29:AG31" si="1">AE28</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AG29">
+        <f>AF28</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AH29">
+        <v>0</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W29),L$22,L$21,FALSE)</f>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" ref="AM29:AN31" si="2">AL28</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AN29">
+        <f>AM28</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="29">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="G30" s="29">
+        <v>0</v>
+      </c>
+      <c r="H30" s="29">
+        <v>539117.22</v>
+      </c>
+      <c r="I30" s="30"/>
+      <c r="J30" s="29">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="K30" s="29">
+        <v>0</v>
+      </c>
+      <c r="L30" s="29">
+        <v>539117.22</v>
+      </c>
+      <c r="M30" s="30"/>
+      <c r="N30" s="29">
+        <v>2.0431115999999999E-2</v>
+      </c>
+      <c r="O30" s="29">
+        <v>0</v>
+      </c>
+      <c r="P30" s="29">
+        <v>1.1765669999999999</v>
+      </c>
+      <c r="R30">
+        <v>0.20431115999999999</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>5.882835</v>
+      </c>
+      <c r="W30" s="12">
+        <v>4</v>
+      </c>
+      <c r="X30">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W30),J$22,J$21,FALSE)</f>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="0"/>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="0"/>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AA30">
+        <f>Z29</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W30),K$22,K$21,FALSE)</f>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="1"/>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="1"/>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AH30">
+        <f>AG29</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W30),L$22,L$21,FALSE)</f>
+        <v>0.29515512740172928</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="2"/>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="2"/>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AO30">
+        <f>AN29</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="F31" s="29">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="G31" s="29">
+        <v>0</v>
+      </c>
+      <c r="H31" s="29">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="I31" s="30"/>
+      <c r="J31" s="29">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="K31" s="29">
+        <v>0</v>
+      </c>
+      <c r="L31" s="29">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="M31" s="30"/>
+      <c r="N31" s="29">
+        <v>2.4059423999999999E-2</v>
+      </c>
+      <c r="O31" s="29">
+        <v>0</v>
+      </c>
+      <c r="P31" s="29">
+        <v>1.5255741</v>
+      </c>
+      <c r="R31">
+        <v>0.24059423999999999</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>7.6278705000000002</v>
+      </c>
+      <c r="W31" s="12">
+        <v>5</v>
+      </c>
+      <c r="X31">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W31),J$22,J$21,FALSE)</f>
+        <v>2.7106590681160576E-2</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="0"/>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="0"/>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="AA31">
+        <f>Z30</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AB31">
+        <f>AA30</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AE31" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W31),K$22,K$21,FALSE)</f>
+        <v>3.7855548657894578E-41</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="1"/>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="1"/>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AH31">
+        <f>AG30</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AI31">
+        <f>AH30</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AL31" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$27:$W31),L$22,L$21,FALSE)</f>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="2"/>
+        <v>0.29515512740172928</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="2"/>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AO31">
+        <f>AN30</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AP31">
+        <f>AO30</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="S33" s="14"/>
+      <c r="X33" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE33" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL33" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS33" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT33" s="9"/>
+      <c r="AU33" s="9"/>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="J34" s="25">
+        <f t="array" ref="J34:L38">N48:P52*J17:L17*8760</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="25">
+        <v>0</v>
+      </c>
+      <c r="L34" s="25">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="array" ref="N34:N38">MMULT(X27:AB31,N27:N31)</f>
+        <v>2.1232145809363784E-3</v>
+      </c>
+      <c r="O34">
+        <f t="array" ref="O34:O38">MMULT(AE27:AI31,O27:O31)</f>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="array" ref="P34:P38">MMULT(AL27:AP31,P27:P31)</f>
+        <v>3.6327290206978106E-3</v>
+      </c>
+      <c r="R34">
+        <f t="array" ref="R34:T38">MMULT(J27:L31,_xlfn.MUNIT(3)*J15:L15)</f>
+        <v>1085.7763</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>508022.2</v>
+      </c>
+      <c r="W34">
+        <f>J21-J20</f>
+        <v>3</v>
+      </c>
+      <c r="X34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$34:$W34)+$W$34,J$22,J$21,FALSE)</f>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="AD34">
+        <f>K21-K20</f>
+        <v>2</v>
+      </c>
+      <c r="AE34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD34)+$AD$34,K$22,K$21,FALSE)</f>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AK34">
+        <f>L21-L20</f>
+        <v>2</v>
+      </c>
+      <c r="AL34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK34)+$AK$34,L$22,L$21,FALSE)</f>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AS34" cm="1">
+        <f t="array" ref="AS34:AS38">X34:X38</f>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="AT34" cm="1">
+        <f t="array" ref="AT34:AT38">AE34:AE38</f>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AU34" cm="1">
+        <f t="array" ref="AU34:AU38">AL34:AL38</f>
+        <v>0.11990416322625341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="J35" s="25">
+        <v>0</v>
+      </c>
+      <c r="K35" s="25">
+        <v>0</v>
+      </c>
+      <c r="L35" s="25">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>7.7637320794872689E-3</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>5.8324395732723237E-2</v>
+      </c>
+      <c r="R35">
+        <v>1302.9315999999999</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>518182.64</v>
+      </c>
+      <c r="W35">
+        <f>W34+1</f>
+        <v>4</v>
+      </c>
+      <c r="X35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$34:$W35)+$W$34,J$22,J$21,FALSE)</f>
+        <v>2.7106590681160576E-2</v>
+      </c>
+      <c r="AD35">
+        <f>AD34+1</f>
+        <v>3</v>
+      </c>
+      <c r="AE35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD35)+$AD$34,K$22,K$21,FALSE)</f>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AK35">
+        <f>AK34+1</f>
+        <v>3</v>
+      </c>
+      <c r="AL35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK35)+$AK$34,L$22,L$21,FALSE)</f>
+        <v>0.29515512740172928</v>
+      </c>
+      <c r="AS35">
+        <v>2.7106590681160576E-2</v>
+      </c>
+      <c r="AT35">
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AU35">
+        <v>0.29515512740172928</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="J36" s="25">
+        <v>0</v>
+      </c>
+      <c r="K36" s="25">
+        <v>0</v>
+      </c>
+      <c r="L36" s="25">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1.2863370967680761E-2</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0.28573344178655952</v>
+      </c>
+      <c r="R36">
+        <v>1563.5178999999998</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="W36">
+        <f t="shared" ref="W36:W38" si="3">W35+1</f>
+        <v>5</v>
+      </c>
+      <c r="X36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$34:$W36)+$W$34,J$22,J$21,FALSE)</f>
+        <v>1.3418505116100498E-3</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" ref="AD36:AD38" si="4">AD35+1</f>
+        <v>4</v>
+      </c>
+      <c r="AE36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD36)+$AD$34,K$22,K$21,FALSE)</f>
+        <v>3.7855548657894578E-41</v>
+      </c>
+      <c r="AK36">
+        <f t="shared" ref="AK36:AK38" si="5">AK35+1</f>
+        <v>4</v>
+      </c>
+      <c r="AL36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK36)+$AK$34,L$22,L$21,FALSE)</f>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="AS36">
+        <v>1.3418505116100498E-3</v>
+      </c>
+      <c r="AT36">
+        <v>3.7855548657894578E-41</v>
+      </c>
+      <c r="AU36">
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="J37" s="25">
+        <v>0</v>
+      </c>
+      <c r="K37" s="25">
+        <v>0</v>
+      </c>
+      <c r="L37" s="25">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>1.5296166457125473E-2</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0.74835119037363873</v>
+      </c>
+      <c r="R37">
+        <v>1878.3931000000002</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>539117.22</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="X37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$34:$W37)+$W$34,J$22,J$21,FALSE)</f>
+        <v>1.6550272633902514E-5</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AE37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD37)+$AD$34,K$22,K$21,FALSE)</f>
+        <v>5.9274230554426089E-104</v>
+      </c>
+      <c r="AK37">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AL37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK37)+$AK$34,L$22,L$21,FALSE)</f>
+        <v>0.17221117858191715</v>
+      </c>
+      <c r="AS37">
+        <v>1.6550272633902514E-5</v>
+      </c>
+      <c r="AT37">
+        <v>5.9274230554426089E-104</v>
+      </c>
+      <c r="AU37">
+        <v>0.17221117858191715</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="J38" s="25">
+        <v>0</v>
+      </c>
+      <c r="K38" s="25">
+        <v>0</v>
+      </c>
+      <c r="L38" s="25">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>1.8039137683535714E-2</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>1.0961515987704216</v>
+      </c>
+      <c r="R38">
+        <v>2247.5569999999998</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="X38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($W$34:$W38)+$W$34,J$22,J$21,FALSE)</f>
+        <v>4.1345408690430844E-8</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AE38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD38)+$AD$34,K$22,K$21,FALSE)</f>
+        <v>2.9826841676640016E-226</v>
+      </c>
+      <c r="AK38">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AL38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK38)+$AK$34,L$22,L$21,FALSE)</f>
+        <v>1.7732590637651324E-2</v>
+      </c>
+      <c r="AS38">
+        <v>4.1345408690430844E-8</v>
+      </c>
+      <c r="AT38">
+        <v>2.9826841676640016E-226</v>
+      </c>
+      <c r="AU38">
+        <v>1.7732590637651324E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="N40" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f t="array" ref="J41:L45">N48:P52*J18:L18*8760</f>
+        <v>108.57763413769814</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>593481.89423281339</v>
+      </c>
+      <c r="N41">
+        <f t="array" ref="N41:P45">J19:L19*AS34:AU38</f>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0.11990416322625341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>130.29316119028221</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>719805.9948692231</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0.29515512740172928</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>156.35179443646376</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>859074.6034414547</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>187.83930503337032</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>964269.4117755451</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0.17221117858191715</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>224.75570072592933</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>1042610.9838706838</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>1.7732590637651324E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="X46" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
+      <c r="X47" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z47" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA47" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB47" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <f t="array" ref="N48:P52">J19:L19-MMULT(X48:AB52,N34:P38)+MMULT(X48:AB52,N27:P31)+MMULT(X48:AB52,N41:P45)</f>
+        <v>1.7706724419063624E-2</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>3.3874537342055557</v>
+      </c>
+      <c r="X48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <v>2.1248069339576355E-2</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>4.1084817058745617</v>
+      </c>
+      <c r="X49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="N50">
+        <v>2.5497683371895591E-2</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>4.9033938552594449</v>
+      </c>
+      <c r="X50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="N51">
+        <v>3.0632632914770114E-2</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>5.5038208434677234</v>
+      </c>
+      <c r="X51" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="N52">
+        <v>3.6652919231234399E-2</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>5.9509759353349532</v>
+      </c>
+      <c r="X52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="N47:S47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
case 3 without discounting and disposal working
</commit_message>
<xml_diff>
--- a/default/3_sut_multi_year_rcot_cap/concept.xlsx
+++ b/default/3_sut_multi_year_rcot_cap/concept.xlsx
@@ -8,160 +8,210 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3_sut_multi_year_rcot_cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C134AB13-0B9A-40D6-A6CE-81B84A79D127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57740533-B7D6-4DD6-8D33-135559005B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no disposal" sheetId="2" r:id="rId1"/>
-    <sheet name="disposal_mat" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="disposal_mat" sheetId="3" r:id="rId2"/>
     <sheet name="disposal" sheetId="4" r:id="rId3"/>
+    <sheet name="discounting" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="3" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="3" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="3" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="3" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">discounting!$F$27:$H$31,discounting!$N$27:$P$31,discounting!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">disposal!$F$27:$H$31,disposal!$N$27:$P$31,disposal!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31,disposal_mat!$N$27:$P$31,disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28,'no disposal'!$N$24:$P$28,'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">discounting!$Z$10:$AD$12</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">disposal!$Z$10:$AD$12</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">disposal_mat!$AD$10:$AH$12</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'no disposal'!$Z$10:$AD$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">discounting!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">disposal!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">disposal_mat!$F$27:$H$31</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'no disposal'!$F$24:$H$28</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">discounting!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">discounting!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">disposal!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">disposal_mat!$J$34:$L$38</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'no disposal'!$J$32:$L$36</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">discounting!$Z$7:$AD$8</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">disposal!$Z$7:$AD$8</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">disposal_mat!$AD$7:$AH$8</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'no disposal'!$Z$7:$AD$8</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">discounting!$J$27:$L$31</definedName>
     <definedName name="solver_lhs6" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
     <definedName name="solver_lhs6" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">discounting!$T$14</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">disposal!$T$14</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">disposal_mat!$X$14</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'no disposal'!$T$14</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">discounting!$J$41:$L$45</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">disposal!$J$41:$L$45</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">disposal_mat!$J$41:$L$45</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'no disposal'!$J$39:$L$43</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">discounting!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">disposal!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">disposal_mat!$J$27:$L$31</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'no disposal'!$J$24:$L$28</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -209,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="109">
   <si>
     <t>time</t>
   </si>
@@ -521,6 +571,21 @@
   </si>
   <si>
     <t>Cap_op = c_start + Tyy*Cap_new + Tyy*Cap_disp_new + Tyy*Cap_disp_start</t>
+  </si>
+  <si>
+    <t>dr</t>
+  </si>
+  <si>
+    <t>Minimize(sum(C_inv_y,C_om_y))</t>
+  </si>
+  <si>
+    <t>C_inv_y = C_inv/(1+dr)^(years-1)</t>
+  </si>
+  <si>
+    <t>C_om_y = C_om/(1+dr)^(years-1)</t>
+  </si>
+  <si>
+    <t>Cap_disp_start = c_start*  weib_concat</t>
   </si>
 </sst>
 </file>
@@ -681,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -717,8 +782,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1004,32 +1068,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43994AB8-4797-4F82-A05D-BD00A3481ACB}">
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="12" width="6.85546875" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="16" width="7.42578125" customWidth="1"/>
-    <col min="17" max="18" width="6.28515625" customWidth="1"/>
-    <col min="19" max="19" width="4.85546875" customWidth="1"/>
-    <col min="20" max="30" width="7.42578125" customWidth="1"/>
-    <col min="31" max="32" width="4.85546875" customWidth="1"/>
-    <col min="33" max="33" width="5.28515625" customWidth="1"/>
-    <col min="34" max="36" width="7.140625" customWidth="1"/>
-    <col min="37" max="41" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.453125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="12" width="6.81640625" customWidth="1"/>
+    <col min="13" max="13" width="4.7265625" customWidth="1"/>
+    <col min="14" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="18" width="6.26953125" customWidth="1"/>
+    <col min="19" max="19" width="4.81640625" customWidth="1"/>
+    <col min="20" max="30" width="7.453125" customWidth="1"/>
+    <col min="31" max="32" width="4.81640625" customWidth="1"/>
+    <col min="33" max="33" width="5.26953125" customWidth="1"/>
+    <col min="34" max="36" width="7.1796875" customWidth="1"/>
+    <col min="37" max="41" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1128,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1078,7 +1142,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -1092,12 +1156,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -1126,7 +1190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J6" s="14" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1213,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
@@ -1307,7 +1371,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -1348,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -1388,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -1428,12 +1492,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="T13" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>16</v>
       </c>
@@ -1460,7 +1524,7 @@
         <v>2651862.165910033</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>17</v>
       </c>
@@ -1480,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>19</v>
       </c>
@@ -1500,7 +1564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -1520,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
         <v>30</v>
       </c>
@@ -1537,7 +1601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>48</v>
       </c>
@@ -1557,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="F22" s="14" t="s">
         <v>31</v>
       </c>
@@ -1572,7 +1636,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
         <v>50</v>
       </c>
@@ -1610,7 +1674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1716,7 @@
         <v>14.498350499999999</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1693,7 +1757,7 @@
         <v>0.28996701000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1734,7 +1798,7 @@
         <v>0.29576635000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1775,7 +1839,7 @@
         <v>0.30168167499999998</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1816,7 +1880,7 @@
         <v>0.30771531000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J31" s="14" t="s">
         <v>40</v>
       </c>
@@ -1834,7 +1898,7 @@
       </c>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1869,7 +1933,7 @@
         <v>508022.2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1901,7 +1965,7 @@
         <v>518182.64</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1933,7 +1997,7 @@
         <v>528546.30000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1965,7 +2029,7 @@
         <v>539117.22</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1997,12 +2061,12 @@
         <v>549899.56999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J38" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2081,7 @@
         <v>508022.20151999994</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -2031,7 +2095,7 @@
         <v>518182.64555039996</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -2045,7 +2109,7 @@
         <v>528546.29845440004</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -2059,7 +2123,7 @@
         <v>539117.22434640001</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -2073,12 +2137,12 @@
         <v>549899.56880879996</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="N45" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2098,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -2118,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -2138,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>27</v>
       </c>
@@ -2158,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -2192,32 +2256,32 @@
       <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
+      <selection pane="bottomRight" activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="12" width="6.85546875" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="16" width="7.42578125" customWidth="1"/>
-    <col min="17" max="18" width="6.28515625" customWidth="1"/>
-    <col min="19" max="19" width="4.85546875" customWidth="1"/>
-    <col min="20" max="32" width="7.42578125" customWidth="1"/>
-    <col min="33" max="34" width="4.85546875" customWidth="1"/>
-    <col min="35" max="35" width="5.28515625" customWidth="1"/>
-    <col min="36" max="38" width="7.140625" customWidth="1"/>
-    <col min="39" max="43" width="5.28515625" customWidth="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.453125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="12" width="6.81640625" customWidth="1"/>
+    <col min="13" max="13" width="4.7265625" customWidth="1"/>
+    <col min="14" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="18" width="6.26953125" customWidth="1"/>
+    <col min="19" max="19" width="4.81640625" customWidth="1"/>
+    <col min="20" max="32" width="7.453125" customWidth="1"/>
+    <col min="33" max="34" width="4.81640625" customWidth="1"/>
+    <col min="35" max="35" width="5.26953125" customWidth="1"/>
+    <col min="36" max="38" width="7.1796875" customWidth="1"/>
+    <col min="39" max="43" width="5.26953125" customWidth="1"/>
+    <col min="46" max="46" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +2316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>81</v>
       </c>
@@ -2266,7 +2330,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -2280,12 +2344,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="73.5" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -2306,7 +2370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="J6" s="14" t="s">
         <v>9</v>
       </c>
@@ -2329,7 +2393,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -2479,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
@@ -2487,7 +2551,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -2528,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -2568,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -2608,12 +2672,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="X13" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>16</v>
       </c>
@@ -2640,7 +2704,7 @@
         <v>2651877.8847193602</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>17</v>
       </c>
@@ -2660,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>19</v>
       </c>
@@ -2680,7 +2744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -2700,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
         <v>30</v>
       </c>
@@ -2717,7 +2781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>48</v>
       </c>
@@ -2737,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>66</v>
       </c>
@@ -2757,7 +2821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>65</v>
       </c>
@@ -2777,7 +2841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>63</v>
       </c>
@@ -2797,7 +2861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:59" x14ac:dyDescent="0.35">
       <c r="X24" s="14" t="s">
         <v>72</v>
       </c>
@@ -2811,7 +2875,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:59" x14ac:dyDescent="0.35">
       <c r="F25" s="14" t="s">
         <v>31</v>
       </c>
@@ -2838,7 +2902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:59" x14ac:dyDescent="0.35">
       <c r="F26" t="s">
         <v>50</v>
       </c>
@@ -2969,7 +3033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3110,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -3250,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3393,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4</v>
       </c>
@@ -3539,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
@@ -3688,7 +3752,7 @@
         <v>1.599488081911263E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:59" x14ac:dyDescent="0.35">
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -3699,7 +3763,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="J33" s="14" t="s">
         <v>40</v>
       </c>
@@ -3727,7 +3791,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3798,7 +3862,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3863,7 +3927,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -3928,7 +3992,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3993,7 +4057,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -4058,7 +4122,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.35">
       <c r="J40" s="14" t="s">
         <v>41</v>
       </c>
@@ -4068,7 +4132,7 @@
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -4093,7 +4157,7 @@
         <v>2.89967012980786</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4116,7 +4180,7 @@
         <v>2.9576635329036942</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3</v>
       </c>
@@ -4139,7 +4203,7 @@
         <v>3.0168167999456923</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>4</v>
       </c>
@@ -4162,7 +4226,7 @@
         <v>3.0771531684006117</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>5</v>
       </c>
@@ -4185,12 +4249,12 @@
         <v>3.1386962284587483</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.35">
       <c r="N47" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
@@ -4210,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4230,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -4250,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>4</v>
       </c>
@@ -4270,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>5</v>
       </c>
@@ -4290,14 +4354,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N54" s="27" t="s">
         <v>80</v>
       </c>
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N55" cm="1">
         <f t="array" ref="N55:N59">N27:N31</f>
         <v>1.9829939000000001E-2</v>
@@ -4309,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N56">
         <v>1.1305077E-2</v>
       </c>
@@ -4320,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N57">
         <v>1.7112985000000001E-2</v>
       </c>
@@ -4331,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N58">
         <v>2.0431115999999999E-2</v>
       </c>
@@ -4342,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N59">
         <v>2.4059423999999999E-2</v>
       </c>
@@ -4353,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N60">
         <v>0</v>
       </c>
@@ -4365,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N61">
         <v>0</v>
       </c>
@@ -4376,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N62">
         <v>0</v>
       </c>
@@ -4387,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N63">
         <v>0</v>
       </c>
@@ -4398,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N64">
         <v>0</v>
       </c>
@@ -4409,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="14:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="14:16" x14ac:dyDescent="0.35">
       <c r="N65">
         <v>0</v>
       </c>
@@ -4421,7 +4485,7 @@
         <v>2.2711823</v>
       </c>
     </row>
-    <row r="66" spans="14:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="14:16" x14ac:dyDescent="0.35">
       <c r="N66">
         <v>0</v>
       </c>
@@ -4432,7 +4496,7 @@
         <v>0.48419723999999997</v>
       </c>
     </row>
-    <row r="67" spans="14:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="14:16" x14ac:dyDescent="0.35">
       <c r="N67">
         <v>0</v>
       </c>
@@ -4443,7 +4507,7 @@
         <v>0.71276614999999999</v>
       </c>
     </row>
-    <row r="68" spans="14:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="14:16" x14ac:dyDescent="0.35">
       <c r="N68">
         <v>0</v>
       </c>
@@ -4454,7 +4518,7 @@
         <v>1.1765669999999999</v>
       </c>
     </row>
-    <row r="69" spans="14:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="14:16" x14ac:dyDescent="0.35">
       <c r="N69">
         <v>0</v>
       </c>
@@ -4474,37 +4538,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F067AF8-4B71-42B5-9201-A885A5FCA9EF}">
   <dimension ref="A1:AU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X24" sqref="X24"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="12" width="6.85546875" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="16" width="7.42578125" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" customWidth="1"/>
-    <col min="18" max="18" width="6.28515625" customWidth="1"/>
-    <col min="19" max="19" width="4.85546875" customWidth="1"/>
-    <col min="20" max="32" width="7.42578125" customWidth="1"/>
-    <col min="33" max="34" width="4.85546875" customWidth="1"/>
-    <col min="35" max="35" width="5.28515625" customWidth="1"/>
-    <col min="36" max="38" width="7.140625" customWidth="1"/>
-    <col min="39" max="43" width="5.28515625" customWidth="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.453125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="12" width="6.81640625" customWidth="1"/>
+    <col min="13" max="13" width="4.7265625" customWidth="1"/>
+    <col min="14" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="17" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.26953125" customWidth="1"/>
+    <col min="19" max="19" width="4.81640625" customWidth="1"/>
+    <col min="20" max="32" width="7.453125" customWidth="1"/>
+    <col min="33" max="34" width="4.81640625" customWidth="1"/>
+    <col min="35" max="35" width="5.26953125" customWidth="1"/>
+    <col min="36" max="38" width="7.1796875" customWidth="1"/>
+    <col min="39" max="43" width="5.26953125" customWidth="1"/>
+    <col min="46" max="46" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4539,7 +4603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>81</v>
       </c>
@@ -4562,7 +4626,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -4575,13 +4639,16 @@
       <c r="L3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="73.5" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -4595,11 +4662,8 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="N5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J6" s="14" t="s">
         <v>9</v>
       </c>
@@ -4616,7 +4680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -4692,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -4766,15 +4830,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="F9" s="14" t="s">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="Z9" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -4815,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -4855,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -4895,12 +4959,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="T13" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>16</v>
       </c>
@@ -4927,7 +4991,7 @@
         <v>2651877.8847193602</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>17</v>
       </c>
@@ -4947,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>19</v>
       </c>
@@ -4967,7 +5031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -4987,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
         <v>30</v>
       </c>
@@ -5004,13 +5068,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>48</v>
       </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
       <c r="I19" s="24" t="s">
         <v>102</v>
       </c>
@@ -5024,7 +5085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>66</v>
       </c>
@@ -5044,7 +5105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>65</v>
       </c>
@@ -5064,7 +5125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>63</v>
       </c>
@@ -5084,7 +5145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="X24" s="14" t="s">
         <v>94</v>
       </c>
@@ -5095,7 +5156,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="F25" s="14" t="s">
         <v>31</v>
       </c>
@@ -5113,7 +5174,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
       <c r="F26" t="s">
         <v>50</v>
       </c>
@@ -5199,37 +5260,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="4">
         <v>108.57763</v>
       </c>
-      <c r="G27" s="29">
-        <v>0</v>
-      </c>
-      <c r="H27" s="29">
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
         <v>508022.2</v>
       </c>
-      <c r="I27" s="30"/>
-      <c r="J27" s="29">
+      <c r="J27" s="4">
         <v>108.57763</v>
       </c>
-      <c r="K27" s="29">
-        <v>0</v>
-      </c>
-      <c r="L27" s="29">
+      <c r="K27" s="4">
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
         <v>508022.2</v>
       </c>
-      <c r="M27" s="30"/>
-      <c r="N27" s="29">
+      <c r="N27" s="4">
         <v>1.9829939000000001E-2</v>
       </c>
-      <c r="O27" s="29">
-        <v>0</v>
-      </c>
-      <c r="P27" s="29">
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
         <v>2.2711823</v>
       </c>
       <c r="R27">
@@ -5294,37 +5353,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="4">
         <v>130.29316</v>
       </c>
-      <c r="G28" s="29">
-        <v>0</v>
-      </c>
-      <c r="H28" s="29">
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
         <v>518182.64</v>
       </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="29">
+      <c r="J28" s="4">
         <v>130.29316</v>
       </c>
-      <c r="K28" s="29">
-        <v>0</v>
-      </c>
-      <c r="L28" s="29">
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
         <v>518182.64</v>
       </c>
-      <c r="M28" s="30"/>
-      <c r="N28" s="29">
+      <c r="N28" s="4">
         <v>1.1305077E-2</v>
       </c>
-      <c r="O28" s="29">
-        <v>0</v>
-      </c>
-      <c r="P28" s="29">
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
         <v>0.48419723999999997</v>
       </c>
       <c r="R28">
@@ -5391,37 +5448,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="4">
         <v>156.35178999999999</v>
       </c>
-      <c r="G29" s="29">
-        <v>0</v>
-      </c>
-      <c r="H29" s="29">
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
         <v>528546.30000000005</v>
       </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="29">
+      <c r="J29" s="4">
         <v>156.35178999999999</v>
       </c>
-      <c r="K29" s="29">
-        <v>0</v>
-      </c>
-      <c r="L29" s="29">
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
         <v>528546.30000000005</v>
       </c>
-      <c r="M29" s="30"/>
-      <c r="N29" s="29">
+      <c r="N29" s="4">
         <v>1.7112985000000001E-2</v>
       </c>
-      <c r="O29" s="29">
-        <v>0</v>
-      </c>
-      <c r="P29" s="29">
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
         <v>0.71276614999999999</v>
       </c>
       <c r="R29">
@@ -5491,37 +5546,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="4">
         <v>187.83931000000001</v>
       </c>
-      <c r="G30" s="29">
-        <v>0</v>
-      </c>
-      <c r="H30" s="29">
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
         <v>539117.22</v>
       </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="29">
+      <c r="J30" s="4">
         <v>187.83931000000001</v>
       </c>
-      <c r="K30" s="29">
-        <v>0</v>
-      </c>
-      <c r="L30" s="29">
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
         <v>539117.22</v>
       </c>
-      <c r="M30" s="30"/>
-      <c r="N30" s="29">
+      <c r="N30" s="4">
         <v>2.0431115999999999E-2</v>
       </c>
-      <c r="O30" s="29">
-        <v>0</v>
-      </c>
-      <c r="P30" s="29">
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
         <v>1.1765669999999999</v>
       </c>
       <c r="R30">
@@ -5594,37 +5647,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="4">
         <v>224.75569999999999</v>
       </c>
-      <c r="G31" s="29">
-        <v>0</v>
-      </c>
-      <c r="H31" s="29">
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
         <v>549899.56999999995</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="29">
+      <c r="J31" s="4">
         <v>224.75569999999999</v>
       </c>
-      <c r="K31" s="29">
-        <v>0</v>
-      </c>
-      <c r="L31" s="29">
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
         <v>549899.56999999995</v>
       </c>
-      <c r="M31" s="30"/>
-      <c r="N31" s="29">
+      <c r="N31" s="4">
         <v>2.4059423999999999E-2</v>
       </c>
-      <c r="O31" s="29">
-        <v>0</v>
-      </c>
-      <c r="P31" s="29">
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4">
         <v>1.5255741</v>
       </c>
       <c r="R31">
@@ -5700,7 +5751,7 @@
         <v>1.599488081911263E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -5711,18 +5762,18 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="31" t="s">
+    <row r="33" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
       <c r="M33" s="14"/>
-      <c r="N33" s="31" t="s">
+      <c r="N33" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="14" t="s">
         <v>91</v>
@@ -5743,7 +5794,7 @@
       <c r="AT33" s="9"/>
       <c r="AU33" s="9"/>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -5816,7 +5867,7 @@
         <v>0.11990416322625341</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -5881,7 +5932,7 @@
         <v>0.29515512740172928</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -5946,7 +5997,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -6011,7 +6062,7 @@
         <v>0.17221117858191715</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -6076,19 +6127,19 @@
         <v>1.7732590637651324E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="31" t="s">
+    <row r="40" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="N40" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-    </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="N40" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -6113,7 +6164,7 @@
         <v>0.11990416322625341</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -6136,7 +6187,7 @@
         <v>0.29515512740172928</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3</v>
       </c>
@@ -6159,7 +6210,7 @@
         <v>0.36787944117144233</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>4</v>
       </c>
@@ -6182,7 +6233,7 @@
         <v>0.17221117858191715</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>5</v>
       </c>
@@ -6205,20 +6256,20 @@
         <v>1.7732590637651324E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.35">
       <c r="X46" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N47" s="31" t="s">
+    <row r="47" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N47" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="31"/>
-      <c r="S47" s="31"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
       <c r="X47" s="9">
         <v>1</v>
       </c>
@@ -6235,7 +6286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
@@ -6265,7 +6316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
@@ -6294,7 +6345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -6323,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>4</v>
       </c>
@@ -6352,7 +6403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>5</v>
       </c>
@@ -6391,4 +6442,1985 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A526CD-DE21-40CC-88A4-8C9263AC5352}">
+  <dimension ref="A1:AW52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="U7" sqref="U7:U8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.453125" customWidth="1"/>
+    <col min="9" max="9" width="4.7265625" customWidth="1"/>
+    <col min="10" max="12" width="6.81640625" customWidth="1"/>
+    <col min="13" max="13" width="4.7265625" customWidth="1"/>
+    <col min="14" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="17" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.26953125" customWidth="1"/>
+    <col min="19" max="19" width="4.81640625" customWidth="1"/>
+    <col min="20" max="21" width="7.453125" customWidth="1"/>
+    <col min="22" max="23" width="5.7265625" customWidth="1"/>
+    <col min="24" max="24" width="6.7265625" customWidth="1"/>
+    <col min="25" max="32" width="7.453125" customWidth="1"/>
+    <col min="33" max="34" width="4.81640625" customWidth="1"/>
+    <col min="35" max="35" width="5.26953125" customWidth="1"/>
+    <col min="36" max="38" width="7.1796875" customWidth="1"/>
+    <col min="39" max="43" width="5.26953125" customWidth="1"/>
+    <col min="46" max="46" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>2</v>
+      </c>
+      <c r="P1">
+        <v>3</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>5</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <v>2</v>
+      </c>
+      <c r="V1">
+        <v>3</v>
+      </c>
+      <c r="W1">
+        <v>4</v>
+      </c>
+      <c r="X1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="J6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF6" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>100</v>
+      </c>
+      <c r="O7" s="3">
+        <v>120</v>
+      </c>
+      <c r="P7" s="3">
+        <v>144</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>173</v>
+      </c>
+      <c r="R7" s="3">
+        <v>207</v>
+      </c>
+      <c r="T7">
+        <f t="array" ref="T7:X8">MMULT(AF7:AH8,TRANSPOSE(F27:H31))</f>
+        <v>108.57763</v>
+      </c>
+      <c r="U7">
+        <v>130.29316</v>
+      </c>
+      <c r="V7">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="W7">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="X7">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="Z7" s="13">
+        <f t="array" ref="Z7:AD8">T7:X8-MMULT(J7:L8,TRANSPOSE(J27:L31))-N7:R8</f>
+        <v>-2.7699999947117249E-6</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>3.6000000136482413E-7</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>-1.4100000100825127E-6</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>4.5099999965714233E-6</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>-3.0000001061125658E-7</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>508022.19999999995</v>
+      </c>
+      <c r="O8" s="3">
+        <v>518182.64399999997</v>
+      </c>
+      <c r="P8" s="3">
+        <v>528546.29687999992</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>539117.22281759989</v>
+      </c>
+      <c r="R8" s="3">
+        <v>549899.56727395195</v>
+      </c>
+      <c r="T8">
+        <v>508022.2</v>
+      </c>
+      <c r="U8">
+        <v>518182.64</v>
+      </c>
+      <c r="V8">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="W8">
+        <v>539117.22</v>
+      </c>
+      <c r="X8">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>-3.9999999571591616E-3</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>3.1200001249089837E-3</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>-2.8175999177619815E-3</v>
+      </c>
+      <c r="AD8" s="10">
+        <v>2.7260479982942343E-3</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Z10" s="5">
+        <f t="array" ref="Z10:AD12">TRANSPOSE(J27:L31)-MMULT(F10:H12,TRANSPOSE(F27:H31))</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Z11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Z12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="T13" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="2">
+        <v>10</v>
+      </c>
+      <c r="K14" s="2">
+        <v>10</v>
+      </c>
+      <c r="L14" s="2">
+        <v>5</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="T14" s="15">
+        <f>SUM(V27:X31,V34:X38)</f>
+        <v>2406279.7255936628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="2">
+        <v>10</v>
+      </c>
+      <c r="K15" s="2">
+        <v>10</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="2">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
+        <v>5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="2">
+        <v>3</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="2">
+        <v>3</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="AE24" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL24" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS24" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="V25" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE25" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>11</v>
+      </c>
+      <c r="O26" t="s">
+        <v>18</v>
+      </c>
+      <c r="P26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R26" t="s">
+        <v>11</v>
+      </c>
+      <c r="S26" t="s">
+        <v>18</v>
+      </c>
+      <c r="T26" t="s">
+        <v>35</v>
+      </c>
+      <c r="V26" t="s">
+        <v>11</v>
+      </c>
+      <c r="W26" t="s">
+        <v>18</v>
+      </c>
+      <c r="X26" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE26" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI26" s="9">
+        <v>5</v>
+      </c>
+      <c r="AL26" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM26" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP26" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS26" s="9">
+        <v>1</v>
+      </c>
+      <c r="AT26" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU26" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV26" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW26" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>108.57763</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>508022.2</v>
+      </c>
+      <c r="J27" s="4">
+        <v>108.57763</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
+        <v>508022.2</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1.9829939000000001E-2</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
+        <v>1.7826172</v>
+      </c>
+      <c r="R27" s="29">
+        <f t="array" ref="R27:T31">MMULT(N27:P31,_xlfn.MUNIT(3)*J14:L14)</f>
+        <v>0.19829939000000002</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>8.9130859999999998</v>
+      </c>
+      <c r="V27">
+        <f t="array" ref="V27:X31">R27:T31/((1+N10)^(A27:A31-1))</f>
+        <v>0.19829939000000002</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>8.9130859999999998</v>
+      </c>
+      <c r="AD27" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD27),J$22,J$21,FALSE)</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="5">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD27),K$22,K$21,FALSE)</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="5">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD27),L$22,L$21,FALSE)</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AT27">
+        <v>0</v>
+      </c>
+      <c r="AU27">
+        <v>0</v>
+      </c>
+      <c r="AV27">
+        <v>0</v>
+      </c>
+      <c r="AW27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>130.29316</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>518182.64</v>
+      </c>
+      <c r="J28" s="4">
+        <v>130.29316</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>518182.64</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1.1305077E-2</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0.11305076999999999</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0.1076674</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="12">
+        <v>2</v>
+      </c>
+      <c r="AE28">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD28),J$22,J$21,FALSE)</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AF28">
+        <f>AE27</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AG28">
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD28),K$22,K$21,FALSE)</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AM28">
+        <f>AL27</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AN28">
+        <v>0</v>
+      </c>
+      <c r="AO28">
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <v>0</v>
+      </c>
+      <c r="AS28" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD28),L$22,L$21,FALSE)</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AT28">
+        <f>AS27</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AU28">
+        <v>0</v>
+      </c>
+      <c r="AV28">
+        <v>0</v>
+      </c>
+      <c r="AW28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="J29" s="4">
+        <v>156.35178999999999</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="N29" s="4">
+        <v>1.7112985000000001E-2</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0.17112985</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0.1552198185941043</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE29">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD29),J$22,J$21,FALSE)</f>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" ref="AF29:AG31" si="0">AE28</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AG29">
+        <f>AF28</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AH29">
+        <v>0</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD29),K$22,K$21,FALSE)</f>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" ref="AM29:AN31" si="1">AL28</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AN29">
+        <f>AM28</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <v>0</v>
+      </c>
+      <c r="AS29" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD29),L$22,L$21,FALSE)</f>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AT29">
+        <f t="shared" ref="AT29:AU31" si="2">AS28</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AU29">
+        <f>AT28</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AV29">
+        <v>0</v>
+      </c>
+      <c r="AW29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>539117.22</v>
+      </c>
+      <c r="J30" s="4">
+        <v>187.83931000000001</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>539117.22</v>
+      </c>
+      <c r="N30" s="4">
+        <v>2.0431115999999999E-2</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0.12750311</v>
+      </c>
+      <c r="R30">
+        <v>0.20431115999999999</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0.63751555000000004</v>
+      </c>
+      <c r="V30">
+        <v>0.17649166180758014</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0.55070990173847312</v>
+      </c>
+      <c r="AD30" s="12">
+        <v>4</v>
+      </c>
+      <c r="AE30">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD30),J$22,J$21,FALSE)</f>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="0"/>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="0"/>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AH30">
+        <f>AG29</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD30),K$22,K$21,FALSE)</f>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="1"/>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="1"/>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AO30">
+        <f>AN29</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD30),L$22,L$21,FALSE)</f>
+        <v>0.29515512740172928</v>
+      </c>
+      <c r="AT30">
+        <f t="shared" si="2"/>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AU30">
+        <f t="shared" si="2"/>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AV30">
+        <f>AU29</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+      <c r="AW30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="F31" s="4">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="J31" s="4">
+        <v>224.75569999999999</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="N31" s="4">
+        <v>2.4059423999999999E-2</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4">
+        <v>0.70395549000000002</v>
+      </c>
+      <c r="R31">
+        <v>0.24059423999999999</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>3.5197774500000003</v>
+      </c>
+      <c r="V31">
+        <v>0.19793747666867198</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>2.8957296188316599</v>
+      </c>
+      <c r="AD31" s="12">
+        <v>5</v>
+      </c>
+      <c r="AE31">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD31),J$22,J$21,FALSE)</f>
+        <v>2.7106590681160576E-2</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="0"/>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="0"/>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="AH31">
+        <f>AG30</f>
+        <v>0.33047425742484726</v>
+      </c>
+      <c r="AI31">
+        <f>AH30</f>
+        <v>0.10707116047792069</v>
+      </c>
+      <c r="AL31" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD31),K$22,K$21,FALSE)</f>
+        <v>3.7855548657894578E-41</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="1"/>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="1"/>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AO31">
+        <f>AN30</f>
+        <v>0.91969860292860572</v>
+      </c>
+      <c r="AP31">
+        <f>AO30</f>
+        <v>0.15144269288692877</v>
+      </c>
+      <c r="AS31" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$27:$AD31),L$22,L$21,FALSE)</f>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="AT31">
+        <f t="shared" si="2"/>
+        <v>0.29515512740172928</v>
+      </c>
+      <c r="AU31">
+        <f t="shared" si="2"/>
+        <v>0.11990416322625341</v>
+      </c>
+      <c r="AV31">
+        <f>AU30</f>
+        <v>2.5339193607685703E-2</v>
+      </c>
+      <c r="AW31">
+        <f>AV30</f>
+        <v>1.599488081911263E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="S33" s="14"/>
+      <c r="V33" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE33" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL33" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS33" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="J34" s="25">
+        <f t="array" ref="J34:L38">N48:P52*J17:L17*8760</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="25">
+        <v>0</v>
+      </c>
+      <c r="L34" s="25">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="array" ref="N34:N38">MMULT(AE27:AI31,N27:N31)</f>
+        <v>2.1232145809363784E-3</v>
+      </c>
+      <c r="O34">
+        <f t="array" ref="O34:O38">MMULT(AL27:AP31,O27:O31)</f>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="array" ref="P34:P38">MMULT(AS27:AW31,P27:P31)</f>
+        <v>2.8512749660100263E-3</v>
+      </c>
+      <c r="R34">
+        <f t="array" ref="R34:T38">MMULT(J27:L31,_xlfn.MUNIT(3)*J15:L15)</f>
+        <v>1085.7763</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>508022.2</v>
+      </c>
+      <c r="V34">
+        <f t="array" ref="V34:X38">R34:T38/((1+N10)^(A34:A38-1))</f>
+        <v>1085.7763</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>508022.2</v>
+      </c>
+      <c r="AD34">
+        <f>J21-J20</f>
+        <v>3</v>
+      </c>
+      <c r="AE34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD34)+$AD$34,J$22,J$21,FALSE)</f>
+        <v>0.1661264181291118</v>
+      </c>
+      <c r="AK34">
+        <f>K21-K20</f>
+        <v>2</v>
+      </c>
+      <c r="AL34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK34)+$AK$34,K$22,K$21,FALSE)</f>
+        <v>6.3735489107332949E-3</v>
+      </c>
+      <c r="AR34">
+        <f>L21-L20</f>
+        <v>2</v>
+      </c>
+      <c r="AS34" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AR$34:$AR34)+$AR$34,L$22,L$21,FALSE)</f>
+        <v>0.11990416322625341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="J35" s="25">
+        <v>0</v>
+      </c>
+      <c r="K35" s="25">
+        <v>0</v>
+      </c>
+      <c r="L35" s="25">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>7.7637320794872689E-3</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>4.5170082359190587E-2</v>
+      </c>
+      <c r="R35">
+        <v>1302.9315999999999</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>518182.64</v>
+      </c>
+      <c r="V35">
+        <v>1240.887238095238</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>493507.2761904762</v>
+      </c>
+      <c r="AD35">
+        <f>AD34+1</f>
+        <v>4</v>
+      </c>
+      <c r="AE35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD35)+$AD$34,J$22,J$21,FALSE)</f>
+        <v>2.7106590681160576E-2</v>
+      </c>
+      <c r="AK35">
+        <f>AK34+1</f>
+        <v>3</v>
+      </c>
+      <c r="AL35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK35)+$AK$34,K$22,K$21,FALSE)</f>
+        <v>5.0656662196376692E-13</v>
+      </c>
+      <c r="AR35">
+        <f>AR34+1</f>
+        <v>3</v>
+      </c>
+      <c r="AS35" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AR$34:$AR35)+$AR$34,L$22,L$21,FALSE)</f>
+        <v>0.29515512740172928</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="J36" s="25">
+        <v>0</v>
+      </c>
+      <c r="K36" s="25">
+        <v>0</v>
+      </c>
+      <c r="L36" s="25">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1.2863370967680761E-2</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0.21374322371872684</v>
+      </c>
+      <c r="R36">
+        <v>1563.5178999999998</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>528546.30000000005</v>
+      </c>
+      <c r="V36">
+        <v>1418.1568253968253</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>479407.07482993201</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" ref="AD36:AD38" si="3">AD35+1</f>
+        <v>5</v>
+      </c>
+      <c r="AE36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD36)+$AD$34,J$22,J$21,FALSE)</f>
+        <v>1.3418505116100498E-3</v>
+      </c>
+      <c r="AK36">
+        <f t="shared" ref="AK36:AK38" si="4">AK35+1</f>
+        <v>4</v>
+      </c>
+      <c r="AL36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK36)+$AK$34,K$22,K$21,FALSE)</f>
+        <v>3.7855548657894578E-41</v>
+      </c>
+      <c r="AR36">
+        <f t="shared" ref="AR36:AR38" si="5">AR35+1</f>
+        <v>4</v>
+      </c>
+      <c r="AS36" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AR$34:$AR36)+$AR$34,L$22,L$21,FALSE)</f>
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="J37" s="25">
+        <v>0</v>
+      </c>
+      <c r="K37" s="25">
+        <v>0</v>
+      </c>
+      <c r="L37" s="25">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>1.5296166457125473E-2</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0.52635254647936558</v>
+      </c>
+      <c r="R37">
+        <v>1878.3931000000002</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>539117.22</v>
+      </c>
+      <c r="V37">
+        <v>1622.6265846020949</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>465709.72465176537</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AE37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD37)+$AD$34,J$22,J$21,FALSE)</f>
+        <v>1.6550272633902514E-5</v>
+      </c>
+      <c r="AK37">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AL37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK37)+$AK$34,K$22,K$21,FALSE)</f>
+        <v>5.9274230554426089E-104</v>
+      </c>
+      <c r="AR37">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AS37" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AR$34:$AR37)+$AR$34,L$22,L$21,FALSE)</f>
+        <v>0.17221117858191715</v>
+      </c>
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="J38" s="25">
+        <v>0</v>
+      </c>
+      <c r="K38" s="25">
+        <v>0</v>
+      </c>
+      <c r="L38" s="25">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>1.8039137683535714E-2</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0.66014501376492418</v>
+      </c>
+      <c r="R38">
+        <v>2247.5569999999998</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>549899.56999999995</v>
+      </c>
+      <c r="V38">
+        <v>1849.0707061358178</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>452403.73712599167</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="AE38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AD$34:$AD38)+$AD$34,J$22,J$21,FALSE)</f>
+        <v>4.1345408690430844E-8</v>
+      </c>
+      <c r="AK38">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AK$34:$AK38)+$AK$34,K$22,K$21,FALSE)</f>
+        <v>2.9826841676640016E-226</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AS38" s="11">
+        <f>_xlfn.WEIBULL.DIST(COUNTA($AR$34:$AR38)+$AR$34,L$22,L$21,FALSE)</f>
+        <v>1.7732590637651324E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="N40" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f t="array" ref="J41:L45">N48:P52*J18:L18*8760</f>
+        <v>108.57763413769814</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>508022.1994631947</v>
+      </c>
+      <c r="N41">
+        <f t="array" ref="N41:N45">J19*AE34:AE38</f>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="array" ref="O41:O45">K19*AL34:AL38</f>
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f t="array" ref="P41:P45">L19*AS34:AS38</f>
+        <v>0.11990416322625341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>130.29316119028221</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>551819.57935464743</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0.29515512740172928</v>
+      </c>
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>156.35179443646376</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>578824.24465236312</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>187.83930503337032</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>539117.22186873027</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0.17221117858191715</v>
+      </c>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>224.75570072592933</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>549899.56718483206</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>1.7732590637651324E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AE46" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N47" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="AE47" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG47" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH47" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI47" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <f t="array" ref="N48:P52">J19:L19-MMULT(AE48:AI52,N34:P38)+MMULT(AE48:AI52,N27:P31)+MMULT(AE48:AI52,N41:P45)</f>
+        <v>1.7706724419063624E-2</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>2.8996700882602435</v>
+      </c>
+      <c r="AE48" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <v>2.1248069339576355E-2</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>3.1496551333027822</v>
+      </c>
+      <c r="AE49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="N50">
+        <v>2.5497683371895591E-2</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>3.3037913507554979</v>
+      </c>
+      <c r="AE50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="N51">
+        <v>3.0632632914770114E-2</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>3.0771530928580493</v>
+      </c>
+      <c r="AE51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="N52">
+        <v>3.6652919231234399E-2</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>3.1386961597307765</v>
+      </c>
+      <c r="AE52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N47:S47"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="N40:P40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>